<commit_message>
Revize casti Realizace Zakladni Deska
</commit_message>
<xml_diff>
--- a/Text/Zdroje/TPX2/TPX_seq_Katherine_cmd.xlsx
+++ b/Text/Zdroje/TPX2/TPX_seq_Katherine_cmd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Diplomka\Text\Zdroje\TPX2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59C73613-F560-4B05-A0EA-93527C341028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05051ECC-F0EF-451A-B119-983F3EEFEC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2116" yWindow="1215" windowWidth="18031" windowHeight="10681" xr2:uid="{753C3088-B8C7-4A63-9E90-9E74AD7475B0}"/>
+    <workbookView xWindow="12021" yWindow="0" windowWidth="12021" windowHeight="12922" xr2:uid="{753C3088-B8C7-4A63-9E90-9E74AD7475B0}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="32">
   <si>
     <t>CMD_ECHO_CHIP_ID</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>!! - ACK</t>
+  </si>
+  <si>
+    <t>THL Katherine</t>
+  </si>
+  <si>
+    <t>CMD_GET_ACQUISITION_SETUP</t>
   </si>
 </sst>
 </file>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39CA806B-FAB7-429B-BD72-1FFA36F65D12}">
-  <dimension ref="A2:K19"/>
+  <dimension ref="A2:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L32" sqref="L32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -684,7 +690,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G17" s="1" t="s">
         <v>23</v>
       </c>
@@ -692,7 +698,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:11" x14ac:dyDescent="0.3">
       <c r="G18" s="1" t="s">
         <v>24</v>
       </c>
@@ -700,12 +706,105 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="7:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:11" x14ac:dyDescent="0.3">
       <c r="J19" t="s">
         <v>29</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G23" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G24" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G25" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G26" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G27" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G28" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>17</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G30" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="6:11" x14ac:dyDescent="0.3">
+      <c r="G32" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G33" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G34" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G35" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G36" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G37" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G38" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G39" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>